<commit_message>
Update data package at: 2024-01-19T18:11:00Z
</commit_message>
<xml_diff>
--- a/data-raw/Nome_UO_antigas.xlsx
+++ b/data-raw/Nome_UO_antigas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26921"/>
   <workbookPr defaultThemeVersion="124226"/>
   <xr:revisionPtr revIDLastSave="0" documentId="11_F5536F03CADC9C5A0780898254D53320810A57E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
@@ -10,10 +10,21 @@
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -434,26 +445,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c170a06b81d8b923cbfe6a63de8ee1c9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="844dfdedaab7989660d9d802f918fcda" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4338ef-addb-4c87-aefe-1895241b335f"/>
@@ -702,8 +693,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F4F70FD-B48D-426A-882C-1E2AF784F4D5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BA0D396-9C01-4FC3-B727-DFAD7F192519}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -711,5 +722,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BA0D396-9C01-4FC3-B727-DFAD7F192519}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F4F70FD-B48D-426A-882C-1E2AF784F4D5}"/>
 </file>
</xml_diff>